<commit_message>
Added EDA and model result findings. data_preprocessor.py modified to handle data leakage.
</commit_message>
<xml_diff>
--- a/reports/tables/value_counts.xlsx
+++ b/reports/tables/value_counts.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="education" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="self_employed" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="no_of_dependents" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="loan_status" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -520,4 +522,134 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>no_of_dependents</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="n">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>673</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>loan_status</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Approved</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Rejected</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1613</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>